<commit_message>
Markitdown for Excel updated
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SmartGit.Demo\textconv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E6AEBB-8162-40CC-9677-662CF4773236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447996D8-EE53-45B0-855B-A3768C215018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{773691DF-F09B-45E2-B0A3-881A5E86F5C5}"/>
   </bookViews>
@@ -103,11 +103,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86015A30-24E3-4A6F-999A-3C13753A97BE}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,14 +477,14 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>3.1</v>
       </c>
       <c r="C3" s="3">
         <f>B3/A3</f>
-        <v>0.77500000000000002</v>
+        <v>1.0333333333333334</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -497,8 +499,20 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>10</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3.44</v>
+      </c>
+      <c r="C5" s="3">
+        <f>B5/A5</f>
+        <v>0.34399999999999997</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C4">
+  <conditionalFormatting sqref="C2:C5">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>